<commit_message>
chore: Update Grind 75 challenge
</commit_message>
<xml_diff>
--- a/note.xlsx
+++ b/note.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2240" yWindow="2240" windowWidth="19200" windowHeight="11170" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -37,7 +37,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -64,8 +64,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0098fb98"/>
-        <bgColor rgb="0098fb98"/>
+        <fgColor rgb="FF98FB98"/>
+        <bgColor rgb="FF98FB98"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD700"/>
+        <bgColor rgb="FFFFD700"/>
       </patternFill>
     </fill>
     <fill>
@@ -87,7 +93,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -95,6 +101,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -460,13 +467,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -518,19 +525,19 @@
           <t>Arrays &amp; Hashing</t>
         </is>
       </c>
-      <c r="B3" s="6" t="inlineStr">
-        <is>
-          <t>product-of-array-except-self</t>
+      <c r="B3" s="7" t="inlineStr">
+        <is>
+          <t>sort-colors</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Use prefix and postfix to compute the results, original use 2 for loop can do it (time complexity: O(n)), but if use the same array to compute (compute prefix then compute the postfix in the same array), can reduce the memory usage to O(1).</t>
+          <t>Use one path iteration to solve the problem in place, use three pointer, l/r/i like the quick sort to partition the array to three part 0, 1, 2 with a single while loop that swap i and l or i and r, time is O(N), space is (1).</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/product-of-array-except-self/description/</t>
+          <t>https://leetcode.com/problems/sort-colors/description/</t>
         </is>
       </c>
     </row>
@@ -540,19 +547,19 @@
           <t>Arrays &amp; Hashing</t>
         </is>
       </c>
-      <c r="B4" s="5" t="inlineStr">
-        <is>
-          <t>contains-duplicate</t>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>product-of-array-except-self</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Can use both HashSets approach (time-O(n), space-O(n)) or Sorting approach (time-O(n), space-O(1)), consider space or time complexity, which one we want to optimize</t>
+          <t>Use prefix and postfix to compute the results, original use 2 for loop can do it (time complexity: O(n)), but if use the same array to compute (compute prefix then compute the postfix in the same array), can reduce the memory usage to O(1).</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/contains-duplicate/description/</t>
+          <t>https://leetcode.com/problems/product-of-array-except-self/description/</t>
         </is>
       </c>
     </row>
@@ -564,17 +571,17 @@
       </c>
       <c r="B5" s="5" t="inlineStr">
         <is>
-          <t>add-binary</t>
+          <t>contains-duplicate</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Basic String operation practice</t>
+          <t>Can use both HashSets approach (time-O(n), space-O(n)) or Sorting approach (time-O(n), space-O(1)), consider space or time complexity, which one we want to optimize</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/add-binary/description/</t>
+          <t>https://leetcode.com/problems/contains-duplicate/description/</t>
         </is>
       </c>
     </row>
@@ -586,17 +593,17 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>majority-element</t>
+          <t>add-binary</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Can use HashMap to solve, but the Boyer Moore String Search Algorithm is very important to keep tracking the counts changed in the process, save many memory usage.</t>
+          <t>Basic String operation practice</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/majority-element/description/</t>
+          <t>https://leetcode.com/problems/add-binary/description/</t>
         </is>
       </c>
     </row>
@@ -608,17 +615,17 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>longest-palindrome</t>
+          <t>majority-element</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Can use both HashMap or Array to solve this problem, but only array may be more efficiently about time and space complexity by reduce the HashMap operation</t>
+          <t>Can use HashMap to solve, but the Boyer Moore String Search Algorithm is very important to keep tracking the counts changed in the process, save many memory usage.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/longest-palindrome/description/</t>
+          <t>https://leetcode.com/problems/majority-element/description/</t>
         </is>
       </c>
     </row>
@@ -630,17 +637,17 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>ransom-note</t>
+          <t>longest-palindrome</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Use HashMap to trace the number of the character, can use arrays instead of HashMaps (early stop), this would be especially helpful if the character set is known to be ASCII or Unicode with a reasonably small range</t>
+          <t>Can use both HashMap or Array to solve this problem, but only array may be more efficiently about time and space complexity by reduce the HashMap operation</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/ransom-note/description/</t>
+          <t>https://leetcode.com/problems/longest-palindrome/description/</t>
         </is>
       </c>
     </row>
@@ -650,41 +657,41 @@
           <t>Arrays &amp; Hashing</t>
         </is>
       </c>
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>valid-anagram</t>
+      <c r="B9" s="5" t="inlineStr">
+        <is>
+          <t>ransom-note</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Hash map approach to only look once when looping the two string and add it to Hash map (time: O(S+T), spaceㄤO(S+T)), or sort the two string first then compare them (time-O(S+T), space-O(?))</t>
+          <t>Use HashMap to trace the number of the character, can use arrays instead of HashMaps (early stop), this would be especially helpful if the character set is known to be ASCII or Unicode with a reasonably small range</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/valid-anagram/description/</t>
+          <t>https://leetcode.com/problems/ransom-note/description/</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Stack</t>
+          <t>Arrays &amp; Hashing</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>valid-parentheses</t>
+          <t>valid-anagram</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Hash map plus Stack data structure, create Hash map for comparison, then push or pop character into Stack, finally return Stack is empty or not</t>
+          <t>Hash map approach to only look once when looping the two string and add it to Hash map (time: O(S+T), spaceㄤO(S+T)), or sort the two string first then compare them (time-O(S+T), space-O(?))</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/valid-parentheses/description/</t>
+          <t>https://leetcode.com/problems/valid-anagram/description/</t>
         </is>
       </c>
     </row>
@@ -694,19 +701,19 @@
           <t>Stack</t>
         </is>
       </c>
-      <c r="B11" s="6" t="inlineStr">
-        <is>
-          <t>min-stack</t>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>valid-parentheses</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Use two stack can do it, use an vanilla stack as normal stack, and use another stack to always store the smallest value for recording min value.</t>
+          <t>Hash map plus Stack data structure, create Hash map for comparison, then push or pop character into Stack, finally return Stack is empty or not</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/min-stack/description/</t>
+          <t>https://leetcode.com/problems/valid-parentheses/description/</t>
         </is>
       </c>
     </row>
@@ -718,17 +725,17 @@
       </c>
       <c r="B12" s="6" t="inlineStr">
         <is>
-          <t>evaluate-reverse-polish-notation</t>
+          <t>min-stack</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Stack to process the String elements, push the numbers into the Stack and if encounter the operation, pop the numbers out to do the operation then push back, time complexity: O(N).</t>
+          <t>Use two stack can do it, use an vanilla stack as normal stack, and use another stack to always store the smallest value for recording min value.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/evaluate-reverse-polish-notation/description/</t>
+          <t>https://leetcode.com/problems/min-stack/description/</t>
         </is>
       </c>
     </row>
@@ -738,41 +745,41 @@
           <t>Stack</t>
         </is>
       </c>
-      <c r="B13" s="5" t="inlineStr">
-        <is>
-          <t>implement-queue-using-stacks</t>
+      <c r="B13" s="6" t="inlineStr">
+        <is>
+          <t>evaluate-reverse-polish-notation</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>One stack first stores the element, and if pop or peek happens, reverse to element into the second stack before pop or peek actions</t>
+          <t>Stack to process the String elements, push the numbers into the Stack and if encounter the operation, pop the numbers out to do the operation then push back, time complexity: O(N).</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/implement-queue-using-stacks/description/</t>
+          <t>https://leetcode.com/problems/evaluate-reverse-polish-notation/description/</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Two Pointers</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="inlineStr">
-        <is>
-          <t>valid-palindrome</t>
+          <t>Stack</t>
+        </is>
+      </c>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>implement-queue-using-stacks</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Two pointer from head and tail, screen the entire array if char is alpha or num, then see if left == right, time: O(n)</t>
+          <t>One stack first stores the element, and if pop or peek happens, reverse to element into the second stack before pop or peek actions</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/valid-palindrome/description/</t>
+          <t>https://leetcode.com/problems/implement-queue-using-stacks/description/</t>
         </is>
       </c>
     </row>
@@ -782,63 +789,63 @@
           <t>Two Pointers</t>
         </is>
       </c>
-      <c r="B15" s="6" t="inlineStr">
-        <is>
-          <t>3sum</t>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>valid-palindrome</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Sort the array first to make the detection of duplicate numbers quicker, then use two pointer technique to find the sum==0, time complexity: O(NlogN) + O(N^2).</t>
+          <t>Two pointer from head and tail, screen the entire array if char is alpha or num, then see if left == right, time: O(n)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/3sum/description/</t>
+          <t>https://leetcode.com/problems/valid-palindrome/description/</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Linked List</t>
-        </is>
-      </c>
-      <c r="B16" s="2" t="inlineStr">
-        <is>
-          <t>merge-two-sorted-lists</t>
+          <t>Two Pointers</t>
+        </is>
+      </c>
+      <c r="B16" s="7" t="inlineStr">
+        <is>
+          <t>container-with-most-water</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Create dummy node (save the head position), screen the two array when they are not None, then link them, finally link the array that is remain, then return dummy node</t>
+          <t>Use two pointers to compute the maxArea, and shift the small height pointer to potentially increase the maxArea. time is O(N), space is O(1).</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/merge-two-sorted-lists/description/</t>
+          <t>https://leetcode.com/problems/container-with-most-water/description/</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Linked List</t>
-        </is>
-      </c>
-      <c r="B17" s="5" t="inlineStr">
-        <is>
-          <t>middle-of-the-linked-list</t>
+          <t>Two Pointers</t>
+        </is>
+      </c>
+      <c r="B17" s="6" t="inlineStr">
+        <is>
+          <t>3sum</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Use slow and fast pointer to find the middle node, be aware of the edge case, time-O(n), space-O(1)</t>
+          <t>Sort the array first to make the detection of duplicate numbers quicker, then use two pointer technique to find the sum==0, time complexity: O(NlogN) + O(N^2).</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/middle-of-the-linked-list/description/</t>
+          <t>https://leetcode.com/problems/3sum/description/</t>
         </is>
       </c>
     </row>
@@ -848,19 +855,19 @@
           <t>Linked List</t>
         </is>
       </c>
-      <c r="B18" s="5" t="inlineStr">
-        <is>
-          <t>reverse-linked-list</t>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>merge-two-sorted-lists</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Can be reversed either iteratively or recursively, the iterative ver. use the two pointer to loop through the entire list and reverse them, the recursive ver. split the problem to the one last node, then back linked the nodes from the end. The T of both method are both O(n), but the M of iterative method is O(1), and the recursive method is O(n)</t>
+          <t>Create dummy node (save the head position), screen the two array when they are not None, then link them, finally link the array that is remain, then return dummy node</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/reverse-linked-list/description/</t>
+          <t>https://leetcode.com/problems/merge-two-sorted-lists/description/</t>
         </is>
       </c>
     </row>
@@ -872,149 +879,149 @@
       </c>
       <c r="B19" s="5" t="inlineStr">
         <is>
-          <t>linked-list-cycle</t>
+          <t>middle-of-the-linked-list</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Floyd's Tortoise and Hare Algorithm use the slow (+1 per cycle) and fast (+2 per cycle) pointer to detect if there is any cycle exist, fast pointer eventually will catch up slow pointer inside n loop, time: O(n), space: O(1)</t>
+          <t>Use slow and fast pointer to find the middle node, be aware of the edge case, time-O(n), space-O(1)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/linked-list-cycle/</t>
+          <t>https://leetcode.com/problems/middle-of-the-linked-list/description/</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Sliding Window</t>
-        </is>
-      </c>
-      <c r="B20" s="2" t="inlineStr">
-        <is>
-          <t>best-time-to-buy-and-sell-stock</t>
+          <t>Linked List</t>
+        </is>
+      </c>
+      <c r="B20" s="5" t="inlineStr">
+        <is>
+          <t>reverse-linked-list</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Two pointer start from 0 and 1, then shift the right pointer, update the profit, then if find the new lowest point, shift left, until right pointer reach the end</t>
+          <t>Can be reversed either iteratively or recursively, the iterative ver. use the two pointer to loop through the entire list and reverse them, the recursive ver. split the problem to the one last node, then back linked the nodes from the end. The T of both method are both O(n), but the M of iterative method is O(1), and the recursive method is O(n)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock/description/</t>
+          <t>https://leetcode.com/problems/reverse-linked-list/description/</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Sliding Window</t>
-        </is>
-      </c>
-      <c r="B21" s="6" t="inlineStr">
-        <is>
-          <t>longest-substring-without-repeating-characters</t>
+          <t>Linked List</t>
+        </is>
+      </c>
+      <c r="B21" s="5" t="inlineStr">
+        <is>
+          <t>linked-list-cycle</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Sliding window plus HashSet to record the longest result, if the duplicate appear, keep popping the  character in the set util it doesn't have any duplicate, and keep the longest result so far.</t>
+          <t>Floyd's Tortoise and Hare Algorithm use the slow (+1 per cycle) and fast (+2 per cycle) pointer to detect if there is any cycle exist, fast pointer eventually will catch up slow pointer inside n loop, time: O(n), space: O(1)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/longest-substring-without-repeating-characters/description/</t>
+          <t>https://leetcode.com/problems/linked-list-cycle/</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Trees</t>
+          <t>Sliding Window</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>invert-binary-tree</t>
+          <t>best-time-to-buy-and-sell-stock</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Recursive switch the left and right node until the node == None</t>
+          <t>Two pointer start from 0 and 1, then shift the right pointer, update the profit, then if find the new lowest point, shift left, until right pointer reach the end</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/invert-binary-tree/description/</t>
+          <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock/description/</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Trees</t>
-        </is>
-      </c>
-      <c r="B23" s="6" t="inlineStr">
-        <is>
-          <t>validate-binary-search-tree</t>
+          <t>Sliding Window</t>
+        </is>
+      </c>
+      <c r="B23" s="7" t="inlineStr">
+        <is>
+          <t>find-all-anagrams-in-a-string</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Use dfs plus passing the lower bound and upper bound for BST checking, recursive check the tree and return the result.</t>
+          <t>Use two pointer sliding window tech to iterate through all the target string, and use dictionary or 26 characters array to compare if they are the same or not. Time is O(M+N). Space is O(1) since only 26 characters.</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/validate-binary-search-tree/description/</t>
+          <t>https://leetcode.com/problems/find-all-anagrams-in-a-string/description/</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Trees</t>
-        </is>
-      </c>
-      <c r="B24" s="6" t="inlineStr">
-        <is>
-          <t>binary-tree-level-order-traversal</t>
+          <t>Sliding Window</t>
+        </is>
+      </c>
+      <c r="B24" s="7" t="inlineStr">
+        <is>
+          <t>longest-palindromic-substring</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Basic BFS can solve the problem by level order traversal.</t>
+          <t>Iterate all the character and with each character, use left and right pointer to check if it was an palindrome, the time is O(N^2), space is O(1).</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/binary-tree-level-order-traversal/description/</t>
+          <t>https://leetcode.com/problems/longest-palindromic-substring/description/</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Trees</t>
-        </is>
-      </c>
-      <c r="B25" s="5" t="inlineStr">
-        <is>
-          <t>subtree-of-another-tree</t>
+          <t>Sliding Window</t>
+        </is>
+      </c>
+      <c r="B25" s="6" t="inlineStr">
+        <is>
+          <t>longest-substring-without-repeating-characters</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Recursive search using the isSameTree helper function (also a recursive search) to search to entire tree, time-O(n*m) because search every node in the main tree with isSameTree function</t>
+          <t>Sliding window plus HashSet to record the longest result, if the duplicate appear, keep popping the  character in the set util it doesn't have any duplicate, and keep the longest result so far.</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/subtree-of-another-tree/description/</t>
+          <t>https://leetcode.com/problems/longest-substring-without-repeating-characters/description/</t>
         </is>
       </c>
     </row>
@@ -1024,19 +1031,19 @@
           <t>Trees</t>
         </is>
       </c>
-      <c r="B26" s="5" t="inlineStr">
-        <is>
-          <t>same-tree</t>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>invert-binary-tree</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Use DFS to check the two tree's root node and recursively check their sub-tree's node is all the same or not</t>
+          <t>Recursive switch the left and right node until the node == None</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/same-tree/description/</t>
+          <t>https://leetcode.com/problems/invert-binary-tree/description/</t>
         </is>
       </c>
     </row>
@@ -1046,19 +1053,19 @@
           <t>Trees</t>
         </is>
       </c>
-      <c r="B27" s="5" t="inlineStr">
-        <is>
-          <t>maximum-depth-of-binary-tree</t>
+      <c r="B27" s="7" t="inlineStr">
+        <is>
+          <t>construct-binary-tree-from-preorder-and-inorder-traversal</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Can be solved using recursive dfs, iterative dfs, iterative bfs, both of those method will achieve time-O(n), space-O(n) in worst case, recursive dfs keep track the max depth of current layer, iterative dfs use stack to keep track the max depth of current layer, and iterative bfs use queue to walk through every layer and increse the depth count (keep offer and poll the node in the queue to track are there any node exist to be processed)</t>
+          <t>Use DFS plus HashMap to get the mid point of tree spliting point (Utilize the preorder and inorder characteristic), and recursive build the entire tree, time is O(N), space is O(N).</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/maximum-depth-of-binary-tree/description/</t>
+          <t>https://leetcode.com/problems/construct-binary-tree-from-preorder-and-inorder-traversal/description/</t>
         </is>
       </c>
     </row>
@@ -1068,19 +1075,19 @@
           <t>Trees</t>
         </is>
       </c>
-      <c r="B28" s="5" t="inlineStr">
-        <is>
-          <t>diameter-of-binary-tree</t>
+      <c r="B28" s="7" t="inlineStr">
+        <is>
+          <t>binary-tree-right-side-view</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Use bottom-up dfs to find the every sub-tree's height and diameter, then recursive call and update the max diameter though global variable, this can achieve time-O(n) complexity</t>
+          <t>Use level-order-traversal (bfs using queue) to go through all the level and update the right side view, time is O(N), space is O(N).</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/diameter-of-binary-tree/description/</t>
+          <t>https://leetcode.com/problems/binary-tree-right-side-view/description/</t>
         </is>
       </c>
     </row>
@@ -1090,19 +1097,19 @@
           <t>Trees</t>
         </is>
       </c>
-      <c r="B29" s="4" t="inlineStr">
-        <is>
-          <t>balanced-binary-tree</t>
+      <c r="B29" s="7" t="inlineStr">
+        <is>
+          <t>lowest-common-ancestor-of-a-binary-tree</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Using dfs to recursive search the tree by dynamic programming, assume the lower level sub tree was balanced, then the upper sub tree need to see whether left and right depth diff &lt;=1, return the boolean is balanced and depth so far every times, until the node == None</t>
+          <t>Recursive dfs search the tree, 3 condition, 1 is a node is another's ancestor, 2 is two node are at different sub-tree, 3 is tree is null, time is O(N), space is O(1) if not counting recursive stack frame, otherwise O(N).</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/balanced-binary-tree/submissions/1209923431/</t>
+          <t>https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-tree/description/</t>
         </is>
       </c>
     </row>
@@ -1112,591 +1119,1053 @@
           <t>Trees</t>
         </is>
       </c>
-      <c r="B30" s="3" t="inlineStr">
-        <is>
-          <t>lowest-common-ancestor-of-a-binary-search-tree</t>
+      <c r="B30" s="6" t="inlineStr">
+        <is>
+          <t>validate-binary-search-tree</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Detect the split point directly, search until the left and right node is not at different tree, time: O(logn), space:O(1)</t>
+          <t>Use dfs plus passing the lower bound and upper bound for BST checking, recursive check the tree and return the result.</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree/description/</t>
+          <t>https://leetcode.com/problems/validate-binary-search-tree/description/</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Binary Search</t>
-        </is>
-      </c>
-      <c r="B31" s="2" t="inlineStr">
-        <is>
-          <t>binary-search</t>
+          <t>Trees</t>
+        </is>
+      </c>
+      <c r="B31" s="6" t="inlineStr">
+        <is>
+          <t>binary-tree-level-order-traversal</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Recursive search the array at mid (left + (right-left)/2) - warning: overfolw, update to mid+1 or mid-1, don't forget to search the left == right condition in the last round, time: O(logn)</t>
+          <t>Basic BFS can solve the problem by level order traversal.</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/binary-search/description/</t>
+          <t>https://leetcode.com/problems/binary-tree-level-order-traversal/description/</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Binary Search</t>
+          <t>Trees</t>
         </is>
       </c>
       <c r="B32" s="5" t="inlineStr">
         <is>
-          <t>first-bad-version</t>
+          <t>subtree-of-another-tree</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Binary search method, use start and end two pointer to move to the mid point where the true value is, be careful for the boundary conditions</t>
+          <t>Recursive search using the isSameTree helper function (also a recursive search) to search to entire tree, time-O(n*m) because search every node in the main tree with isSameTree function</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/first-bad-version/description/</t>
+          <t>https://leetcode.com/problems/subtree-of-another-tree/description/</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Recursive</t>
-        </is>
-      </c>
-      <c r="B33" s="2" t="inlineStr">
-        <is>
-          <t>flood-fill</t>
+          <t>Trees</t>
+        </is>
+      </c>
+      <c r="B33" s="5" t="inlineStr">
+        <is>
+          <t>same-tree</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Recursive search and change the next +1 or -1 pixel and check the boundary condition and color condition</t>
+          <t>Use DFS to check the two tree's root node and recursively check their sub-tree's node is all the same or not</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/flood-fill/description/</t>
+          <t>https://leetcode.com/problems/same-tree/description/</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1-D Dynamic Programming</t>
+          <t>Trees</t>
         </is>
       </c>
       <c r="B34" s="5" t="inlineStr">
         <is>
-          <t>climbing-stairs</t>
+          <t>maximum-depth-of-binary-tree</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Use memory array to perform dynamic programming, setting the initial condition, and iterate through the entire length of 1D array, get the optimal result</t>
+          <t>Can be solved using recursive dfs, iterative dfs, iterative bfs, both of those method will achieve time-O(n), space-O(n) in worst case, recursive dfs keep track the max depth of current layer, iterative dfs use stack to keep track the max depth of current layer, and iterative bfs use queue to walk through every layer and increse the depth count (keep offer and poll the node in the queue to track are there any node exist to be processed)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/climbing-stairs/description/</t>
+          <t>https://leetcode.com/problems/maximum-depth-of-binary-tree/description/</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1-D Dynamic Programming</t>
-        </is>
-      </c>
-      <c r="B35" s="6" t="inlineStr">
-        <is>
-          <t>coin-change</t>
+          <t>Trees</t>
+        </is>
+      </c>
+      <c r="B35" s="5" t="inlineStr">
+        <is>
+          <t>diameter-of-binary-tree</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Dynamic programming by saving the coin combination by dp memory array and iterate through all the dp position, and for both position, find the most minimum combination of coin numbers abd save it, the time complexity is O(amount * len(coins)), space complexity is O(amount) (dp array).</t>
+          <t>Use bottom-up dfs to find the every sub-tree's height and diameter, then recursive call and update the max diameter though global variable, this can achieve time-O(n) complexity</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/coin-change/description/</t>
+          <t>https://leetcode.com/problems/diameter-of-binary-tree/description/</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1-D Dynamic Programming</t>
-        </is>
-      </c>
-      <c r="B36" s="5" t="inlineStr">
-        <is>
-          <t>min-cost-climbing-stairs</t>
+          <t>Trees</t>
+        </is>
+      </c>
+      <c r="B36" s="4" t="inlineStr">
+        <is>
+          <t>balanced-binary-tree</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Dynamic programming to calculate the sum of best choice from the end of the step (create a dummy stair=0 at the end), and finally return the min of 0 or 1, for choose the best starting position</t>
+          <t>Using dfs to recursive search the tree by dynamic programming, assume the lower level sub tree was balanced, then the upper sub tree need to see whether left and right depth diff &lt;=1, return the boolean is balanced and depth so far every times, until the node == None</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/min-cost-climbing-stairs/description/</t>
+          <t>https://leetcode.com/problems/balanced-binary-tree/submissions/1209923431/</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Heap / Priority Queue</t>
-        </is>
-      </c>
-      <c r="B37" s="5" t="inlineStr">
-        <is>
-          <t>kth-largest-element-in-a-stream</t>
+          <t>Trees</t>
+        </is>
+      </c>
+      <c r="B37" s="3" t="inlineStr">
+        <is>
+          <t>lowest-common-ancestor-of-a-binary-search-tree</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>PriorityQueue (heap) to selective store the largest k item, for heapify take time-O(logN), remove the smallest item from the heap take time-O(1)</t>
+          <t>Detect the split point directly, search until the left and right node is not at different tree, time: O(logn), space:O(1)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/kth-largest-element-in-a-stream/description/</t>
+          <t>https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree/description/</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Heap / Priority Queue</t>
-        </is>
-      </c>
-      <c r="B38" s="6" t="inlineStr">
-        <is>
-          <t>k-closest-points-to-origin</t>
+          <t>Binary Search</t>
+        </is>
+      </c>
+      <c r="B38" s="2" t="inlineStr">
+        <is>
+          <t>binary-search</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>MinHeap to maintain the order according to their distance, note that the time complexity is NlogN, even the heap construct should take T(N) (total time complexity is klogN), but in Java it cannot direct construct the heap same time as a comparator argument, so need to add to the heap N time * add operation per time: logN</t>
+          <t>Recursive search the array at mid (left + (right-left)/2) - warning: overfolw, update to mid+1 or mid-1, don't forget to search the left == right condition in the last round, time: O(logn)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/k-closest-points-to-origin/description/</t>
+          <t>https://leetcode.com/problems/binary-search/description/</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Heap / Priority Queue</t>
-        </is>
-      </c>
-      <c r="B39" s="5" t="inlineStr">
-        <is>
-          <t>last-stone-weight</t>
+          <t>Binary Search</t>
+        </is>
+      </c>
+      <c r="B39" s="7" t="inlineStr">
+        <is>
+          <t>time-based-key-value-store</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>MaxHeap to keep popping the stone and push pack the result stone util only one stone left (if there is no stone left, return 0), building a heap take time-O(n), get the largest element and heapify will take time-O(logN), we will do it N time, so the overall time-O(NlogN)</t>
+          <t>Use HashMap to store the key and the list of [timestamp, value] pairs, and use binary search to find the value (because the timestamp will auto increase by default, no need to sort the list every time), the set time is O(1), the get time is O(logN).</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/last-stone-weight/description/</t>
+          <t>https://leetcode.com/problems/time-based-key-value-store/description/</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Bit Manipulation</t>
-        </is>
-      </c>
-      <c r="B40" s="5" t="inlineStr">
-        <is>
-          <t>single-number</t>
+          <t>Binary Search</t>
+        </is>
+      </c>
+      <c r="B40" s="6" t="inlineStr">
+        <is>
+          <t>search-in-rotated-sorted-array</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Using the method that every bit of the same interger added together will result the all 0 bit, so the final result will left only the single number that was alone</t>
+          <t>Use basic binary search, then check the condition that the left side or right side is sorted, if sorted and exist in that range, search this side, if not exist, search the other side.</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/single-number/description/</t>
+          <t>https://leetcode.com/problems/search-in-rotated-sorted-array/description/</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Bit Manipulation</t>
+          <t>Binary Search</t>
         </is>
       </c>
       <c r="B41" s="5" t="inlineStr">
         <is>
-          <t>reverse-bits</t>
+          <t>first-bad-version</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Bits shifting technique to reverse the original bits to a new number's bits, one calculate from left to right, another one calculate from right to left</t>
+          <t>Binary search method, use start and end two pointer to move to the mid point where the true value is, be careful for the boundary conditions</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/reverse-bits/description/</t>
+          <t>https://leetcode.com/problems/first-bad-version/description/</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Bit Manipulation</t>
-        </is>
-      </c>
-      <c r="B42" s="5" t="inlineStr">
-        <is>
-          <t>missing-number</t>
+          <t>Recursive</t>
+        </is>
+      </c>
+      <c r="B42" s="2" t="inlineStr">
+        <is>
+          <t>flood-fill</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Calculate the total sum it should had, then substract it using all the array elements, the result will be the answer</t>
+          <t>Recursive search and change the next +1 or -1 pixel and check the boundary condition and color condition</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/missing-number/description/</t>
+          <t>https://leetcode.com/problems/flood-fill/description/</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Bit Manipulation</t>
+          <t>1-D Dynamic Programming</t>
         </is>
       </c>
       <c r="B43" s="5" t="inlineStr">
         <is>
-          <t>counting-bits</t>
+          <t>climbing-stairs</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Calculate the bit sum using "number-of-1-bits" method to iterate through all the numbers</t>
+          <t>Use memory array to perform dynamic programming, setting the initial condition, and iterate through the entire length of 1D array, get the optimal result</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/counting-bits/description/</t>
+          <t>https://leetcode.com/problems/climbing-stairs/description/</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Bit Manipulation</t>
-        </is>
-      </c>
-      <c r="B44" s="5" t="inlineStr">
-        <is>
-          <t>number-of-1-bits</t>
+          <t>1-D Dynamic Programming</t>
+        </is>
+      </c>
+      <c r="B44" s="7" t="inlineStr">
+        <is>
+          <t>partition-equal-subset-sum</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Bit manipulation using &amp;= operation to calculate n with n-1 (this will reduce a 1 bit per calculation)</t>
+          <t>Use HashSet to store the result of total sum that can be sum up with the different value, and append the each position of the value that can sum up into the Set, time is O(n * target), space(target).</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/number-of-1-bits/description/</t>
+          <t>https://leetcode.com/problems/partition-equal-subset-sum/description/</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Intervals</t>
-        </is>
-      </c>
-      <c r="B45" s="5" t="inlineStr">
-        <is>
-          <t>meeting-rooms</t>
+          <t>1-D Dynamic Programming</t>
+        </is>
+      </c>
+      <c r="B45" s="7" t="inlineStr">
+        <is>
+          <t>word-break</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Sort the time interval base on the start time then compare the end time of the event and the start time of the next event to check if the meeting is not overlaping</t>
+          <t>Use bottom up dynamic programming to solve the problem, from the word tail search that wordDict contain any word that can construct the word and mark as true, if dp[0] mark as true mean that the word can be constructed.time is O(n*m*t) where t is the word matching cost, space is O(n).</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/meeting-rooms/description/</t>
+          <t>https://leetcode.com/problems/word-break/description/</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Intervals</t>
+          <t>1-D Dynamic Programming</t>
         </is>
       </c>
       <c r="B46" s="6" t="inlineStr">
         <is>
-          <t>insert-interval</t>
+          <t>coin-change</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>List data structure to append a interval one at a time (decide to append new one or old one or merge them together), finally return the result, time-O(n)</t>
+          <t>Dynamic programming by saving the coin combination by dp memory array and iterate through all the dp position, and for both position, find the most minimum combination of coin numbers abd save it, the time complexity is O(amount * len(coins)), space complexity is O(amount) (dp array).</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/insert-interval/description/</t>
+          <t>https://leetcode.com/problems/coin-change/description/</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Math &amp; Geometry</t>
+          <t>1-D Dynamic Programming</t>
         </is>
       </c>
       <c r="B47" s="5" t="inlineStr">
         <is>
-          <t>happy-number</t>
+          <t>min-cost-climbing-stairs</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Using HashSet to store the number had calculate and continue calculate the sum of the output of every number, if output = 1 return true, if had already exist in the set (cycle) return false</t>
+          <t>Dynamic programming to calculate the sum of best choice from the end of the step (create a dummy stair=0 at the end), and finally return the min of 0 or 1, for choose the best starting position</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/happy-number/description/</t>
+          <t>https://leetcode.com/problems/min-cost-climbing-stairs/description/</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Math &amp; Geometry</t>
+          <t>Heap / Priority Queue</t>
         </is>
       </c>
       <c r="B48" s="5" t="inlineStr">
         <is>
-          <t>plus-one</t>
+          <t>kth-largest-element-in-a-stream</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Using basic math to carry the digit from end to the start (first create a n+1 array)</t>
+          <t>PriorityQueue (heap) to selective store the largest k item, for heapify take time-O(logN), remove the smallest item from the heap take time-O(1)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/plus-one/description/https://leetcode.com/problems/plus-one/description/</t>
+          <t>https://leetcode.com/problems/kth-largest-element-in-a-stream/description/</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Greedy</t>
+          <t>Heap / Priority Queue</t>
         </is>
       </c>
       <c r="B49" s="6" t="inlineStr">
         <is>
-          <t>maximum-subarray</t>
+          <t>k-closest-points-to-origin</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Two pointer (temp variable) to walk through the entire array, retain the maximum sum of the array (refresh the negative number to 0 before the current position, because it is not contributing to the result)</t>
+          <t>MinHeap to maintain the order according to their distance, note that the time complexity is NlogN, even the heap construct should take T(N) (total time complexity is klogN), but in Java it cannot direct construct the heap same time as a comparator argument, so need to add to the heap N time * add operation per time: logN</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/maximum-subarray/description/</t>
+          <t>https://leetcode.com/problems/k-closest-points-to-origin/description/</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2-D Dynamic Programming</t>
-        </is>
-      </c>
-      <c r="B50" s="6" t="inlineStr">
-        <is>
-          <t>01-matrix</t>
+          <t>Heap / Priority Queue</t>
+        </is>
+      </c>
+      <c r="B50" s="5" t="inlineStr">
+        <is>
+          <t>last-stone-weight</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Can use dfs, bfs, or dynamic programming to solve this problem, take dp as example, calculate from 4 direction and find the minimum path to the 0 of every point, this can be achieve by dp from upper-left to lower-right and from lower-right to upper-left, and minimum the two result to get the shortest path</t>
+          <t>MaxHeap to keep popping the stone and push pack the result stone util only one stone left (if there is no stone left, return 0), building a heap take time-O(n), get the largest element and heapify will take time-O(logN), we will do it N time, so the overall time-O(NlogN)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/01-matrix/description/</t>
+          <t>https://leetcode.com/problems/last-stone-weight/description/</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Graphs</t>
-        </is>
-      </c>
-      <c r="B51" s="6" t="inlineStr">
-        <is>
-          <t>course-schedule</t>
+          <t>Bit Manipulation</t>
+        </is>
+      </c>
+      <c r="B51" s="5" t="inlineStr">
+        <is>
+          <t>single-number</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Use preMap (HashMap&lt;Integer, List&lt;Integer&gt;&gt;) to record the graph structure of the prereq class and do the dfs for all the class and their adj class, then use visitSet to record the current visit class to detect the loop, the time complexity: O(N + P).</t>
+          <t>Using the method that every bit of the same interger added together will result the all 0 bit, so the final result will left only the single number that was alone</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/course-schedule/description/</t>
+          <t>https://leetcode.com/problems/single-number/description/</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Graphs</t>
-        </is>
-      </c>
-      <c r="B52" s="6" t="inlineStr">
-        <is>
-          <t>number-of-islands</t>
+          <t>Bit Manipulation</t>
+        </is>
+      </c>
+      <c r="B52" s="7" t="inlineStr">
+        <is>
+          <t>string-to-integer-atoi</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Use dfs and visited array to discover all the unvisited island, time complexity and space complexity are both O(M*N).</t>
+          <t>Use string parsing tech to dealing all the edge case, time O(N), space is O(1).</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/number-of-islands/description/</t>
+          <t>https://leetcode.com/problems/string-to-integer-atoi/description/</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Graphs</t>
-        </is>
-      </c>
-      <c r="B53" s="6" t="inlineStr">
-        <is>
-          <t>rotting-oranges</t>
+          <t>Bit Manipulation</t>
+        </is>
+      </c>
+      <c r="B53" s="5" t="inlineStr">
+        <is>
+          <t>reverse-bits</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Use bfs to spread the rotten, and also record the fresh orange numbers to monitor if there are any orange not been rotted, the time complexity is O(m*n).</t>
+          <t>Bits shifting technique to reverse the original bits to a new number's bits, one calculate from left to right, another one calculate from right to left</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/rotting-oranges/description/</t>
+          <t>https://leetcode.com/problems/reverse-bits/description/</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Graphs</t>
-        </is>
-      </c>
-      <c r="B54" s="6" t="inlineStr">
-        <is>
-          <t>clone-graph</t>
+          <t>Bit Manipulation</t>
+        </is>
+      </c>
+      <c r="B54" s="5" t="inlineStr">
+        <is>
+          <t>missing-number</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Use HashMap to record which Node had already been maped, and use dfs to walk through all the Node and their neighbors, time complexity is O(E+V).</t>
+          <t>Calculate the total sum it should had, then substract it using all the array elements, the result will be the answer</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/clone-graph/description/</t>
+          <t>https://leetcode.com/problems/missing-number/description/</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Graphs</t>
-        </is>
-      </c>
-      <c r="B55" s="6" t="inlineStr">
-        <is>
-          <t>rotting-oranges</t>
+          <t>Bit Manipulation</t>
+        </is>
+      </c>
+      <c r="B55" s="5" t="inlineStr">
+        <is>
+          <t>counting-bits</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Use dfs strategy to recursive mark the visited island and find the island util all the adj is sea, the time complexity and space complexity is both O(M*N), because we use the extra memory and M*N loop (also each cell is visited only once by DFS -&gt; M*N).</t>
+          <t>Calculate the bit sum using "number-of-1-bits" method to iterate through all the numbers</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/rotting-oranges/description/</t>
+          <t>https://leetcode.com/problems/counting-bits/description/</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
+          <t>Bit Manipulation</t>
+        </is>
+      </c>
+      <c r="B56" s="5" t="inlineStr">
+        <is>
+          <t>number-of-1-bits</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Bit manipulation using &amp;= operation to calculate n with n-1 (this will reduce a 1 bit per calculation)</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/number-of-1-bits/description/</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Intervals</t>
+        </is>
+      </c>
+      <c r="B57" s="5" t="inlineStr">
+        <is>
+          <t>meeting-rooms</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Sort the time interval base on the start time then compare the end time of the event and the start time of the next event to check if the meeting is not overlaping</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/meeting-rooms/description/</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Intervals</t>
+        </is>
+      </c>
+      <c r="B58" s="7" t="inlineStr">
+        <is>
+          <t>merge-intervals</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Sort the intervals first with the start element, and then iterate all the intervals and merge them, time: O(NlogN).</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/merge-intervals/description/</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Intervals</t>
+        </is>
+      </c>
+      <c r="B59" s="6" t="inlineStr">
+        <is>
+          <t>insert-interval</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>List data structure to append a interval one at a time (decide to append new one or old one or merge them together), finally return the result, time-O(n)</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/insert-interval/description/</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Math &amp; Geometry</t>
+        </is>
+      </c>
+      <c r="B60" s="5" t="inlineStr">
+        <is>
+          <t>happy-number</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Using HashSet to store the number had calculate and continue calculate the sum of the output of every number, if output = 1 return true, if had already exist in the set (cycle) return false</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/happy-number/description/</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Math &amp; Geometry</t>
+        </is>
+      </c>
+      <c r="B61" s="7" t="inlineStr">
+        <is>
+          <t>spiral-matrix</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Use boundary plus spiral moving tech to move the point to get all the element, time is O(m * n), space is O(1).</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/spiral-matrix/description/</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Math &amp; Geometry</t>
+        </is>
+      </c>
+      <c r="B62" s="5" t="inlineStr">
+        <is>
+          <t>plus-one</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Using basic math to carry the digit from end to the start (first create a n+1 array)</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/plus-one/description/https://leetcode.com/problems/plus-one/description/</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Greedy</t>
+        </is>
+      </c>
+      <c r="B63" s="6" t="inlineStr">
+        <is>
+          <t>maximum-subarray</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Two pointer (temp variable) to walk through the entire array, retain the maximum sum of the array (refresh the negative number to 0 before the current position, because it is not contributing to the result)</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/maximum-subarray/description/</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2-D Dynamic Programming</t>
+        </is>
+      </c>
+      <c r="B64" s="6" t="inlineStr">
+        <is>
+          <t>01-matrix</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Can use dfs, bfs, or dynamic programming to solve this problem, take dp as example, calculate from 4 direction and find the minimum path to the 0 of every point, this can be achieve by dp from upper-left to lower-right and from lower-right to upper-left, and minimum the two result to get the shortest path</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/01-matrix/description/</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2-D Dynamic Programming</t>
+        </is>
+      </c>
+      <c r="B65" s="7" t="inlineStr">
+        <is>
+          <t>unique-paths</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Use Top-Down dynamic programming to compute the result, can even use space optimization tech to reduce the memory usage to only memo the last row. time is O(M*N), space is O(N).</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/unique-paths/description/</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Graphs</t>
+        </is>
+      </c>
+      <c r="B66" s="6" t="inlineStr">
+        <is>
+          <t>course-schedule</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Use preMap (HashMap&lt;Integer, List&lt;Integer&gt;&gt;) to record the graph structure of the prereq class and do the dfs for all the class and their adj class, then use visitSet to record the current visit class to detect the loop, the time complexity: O(N + P).</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/course-schedule/description/</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Graphs</t>
+        </is>
+      </c>
+      <c r="B67" s="6" t="inlineStr">
+        <is>
+          <t>number-of-islands</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Use dfs and visited array to discover all the unvisited island, time complexity and space complexity are both O(M*N).</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/number-of-islands/description/</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Graphs</t>
+        </is>
+      </c>
+      <c r="B68" s="6" t="inlineStr">
+        <is>
+          <t>rotting-oranges</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Use bfs to spread the rotten, and also record the fresh orange numbers to monitor if there are any orange not been rotted, the time complexity is O(m*n).</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/rotting-oranges/description/</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Graphs</t>
+        </is>
+      </c>
+      <c r="B69" s="6" t="inlineStr">
+        <is>
+          <t>clone-graph</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Use HashMap to record which Node had already been maped, and use dfs to walk through all the Node and their neighbors, time complexity is O(E+V).</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/clone-graph/description/</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Graphs</t>
+        </is>
+      </c>
+      <c r="B70" s="6" t="inlineStr">
+        <is>
+          <t>rotting-oranges</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Use dfs strategy to recursive mark the visited island and find the island util all the adj is sea, the time complexity and space complexity is both O(M*N), because we use the extra memory and M*N loop (also each cell is visited only once by DFS -&gt; M*N).</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/rotting-oranges/description/</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
           <t>Tries</t>
         </is>
       </c>
-      <c r="B56" s="6" t="inlineStr">
+      <c r="B71" s="6" t="inlineStr">
         <is>
           <t>implement-trie-prefix-tree</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="C71" t="inlineStr">
         <is>
           <t>Use tree structure (Node that contain HashMap to record character in this layer and a boolean to record end of the words) staring from the root to record the words that has been added, for adding the new words, iterate through the character of the words, if the character not exist yet, add a new node, and finally mark the end of the words for searching.</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
+      <c r="D71" t="inlineStr">
         <is>
           <t>https://leetcode.com/problems/implement-trie-prefix-tree/description/</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Backtracking</t>
+        </is>
+      </c>
+      <c r="B72" s="7" t="inlineStr">
+        <is>
+          <t>combination-sum</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Use dfs to track the every combination of the elements, if equal -&gt; push into result, if exceed the sum or out of range -&gt; break, then continue search the rest of combination, be aware of the shallow copy that push into the result array, might result in call by reference issue.</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/combination-sum/description/</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Backtracking</t>
+        </is>
+      </c>
+      <c r="B73" s="7" t="inlineStr">
+        <is>
+          <t>word-search</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Use backtracking tech to search every possible 4 direction to build the word, use label to bloack the text that already visited to avoid reuse the text. Time is O(M*4^N). Space is O(N).</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/word-search/description/</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Backtracking</t>
+        </is>
+      </c>
+      <c r="B74" s="7" t="inlineStr">
+        <is>
+          <t>letter-combinations-of-a-phone-number</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Use backtracking and a map to map the number to the string, and find all the solution by  building the entire string. Time is O(N*4^N), Space is O(N).</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/letter-combinations-of-a-phone-number/description/</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Backtracking</t>
+        </is>
+      </c>
+      <c r="B75" s="7" t="inlineStr">
+        <is>
+          <t>subsets</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Use backtracking to store whether to include the current number or skip it, time O(N * 2^N), space is O(N).</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/subsets/description/</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Backtracking</t>
+        </is>
+      </c>
+      <c r="B76" s="7" t="inlineStr">
+        <is>
+          <t>permutations</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Use recursive approach to build the permutations from bottom to top, and insert the one element into the array each step (multiple site insertion), time is O(N! * N^2), space is O(N! * N).</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/permutations/description/</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Union Find</t>
+        </is>
+      </c>
+      <c r="B77" s="7" t="inlineStr">
+        <is>
+          <t>accounts-merge</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Use union find data structure to create mail to index of account and index of account to mail list, the time is O(m*n)log(m*n), the space is (m*n).</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/accounts-merge/description/</t>
         </is>
       </c>
     </row>

</xml_diff>